<commit_message>
changed hours used function
</commit_message>
<xml_diff>
--- a/CFA_Exploration.xlsx
+++ b/CFA_Exploration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datdo\Documents\Bethel\11_FinalProject\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D8D987-E77A-44B0-9840-CD403517FFEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F3EAE1-49E0-4ADE-8AFE-A8CFC6F4050E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="660" windowWidth="23280" windowHeight="14430" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29985" yWindow="960" windowWidth="23280" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot Table" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="34">
   <si>
     <t>Week</t>
   </si>
@@ -128,12 +128,6 @@
     <t>Average of Sales</t>
   </si>
   <si>
-    <t>Sum of HoursUsed</t>
-  </si>
-  <si>
-    <t>Sum of HoursUsed2</t>
-  </si>
-  <si>
     <t>average % sales Before:</t>
   </si>
   <si>
@@ -141,6 +135,9 @@
   </si>
   <si>
     <t>average % sales After:</t>
+  </si>
+  <si>
+    <t>Average of HoursUsed</t>
   </si>
 </sst>
 </file>
@@ -214,9 +211,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
@@ -225,7 +222,19 @@
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1292,8 +1301,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9F5105C-0A0B-4CAF-89F3-B1C2EAECEE58}" name="PivotTable1" cacheId="4" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:E14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9F5105C-0A0B-4CAF-89F3-B1C2EAECEE58}" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1371,7 +1380,7 @@
   <rowFields count="1">
     <field x="-2"/>
   </rowFields>
-  <rowItems count="10">
+  <rowItems count="9">
     <i>
       <x/>
     </i>
@@ -1399,9 +1408,6 @@
     <i i="8">
       <x v="8"/>
     </i>
-    <i i="9">
-      <x v="9"/>
-    </i>
   </rowItems>
   <colFields count="1">
     <field x="15"/>
@@ -1420,8 +1426,7 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="10">
-    <dataField name="Sum of HoursUsed2" fld="2" baseField="15" baseItem="0" numFmtId="4"/>
+  <dataFields count="9">
     <dataField name="Average of Sales" fld="1" subtotal="average" baseField="15" baseItem="0"/>
     <dataField name="Average of CarryO" fld="9" subtotal="average" baseField="15" baseItem="0"/>
     <dataField name="Average of MobCO" fld="3" subtotal="average" baseField="15" baseItem="0"/>
@@ -1430,19 +1435,10 @@
     <dataField name="Average of MobDT" fld="5" subtotal="average" baseField="15" baseItem="0"/>
     <dataField name="Average of NormDT" fld="8" subtotal="average" baseField="15" baseItem="0"/>
     <dataField name="Average of Catering" fld="11" subtotal="average" baseField="15" baseItem="0"/>
-    <dataField name="Sum of HoursUsed" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Average of HoursUsed" fld="2" subtotal="average" baseField="15" baseItem="0"/>
   </dataFields>
-  <formats count="2">
-    <format dxfId="2">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
+  <formats count="1">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1781,17 +1777,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA540E03-21C0-4ACF-978A-4AF1244D8D01}">
   <dimension ref="A3:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="15" width="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
@@ -1847,78 +1843,78 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4">
-        <v>35190.33</v>
+        <v>122075.35210526315</v>
       </c>
       <c r="C5" s="4">
-        <v>7413.92</v>
+        <v>95590.301999999996</v>
       </c>
       <c r="D5" s="4">
-        <v>52205.22</v>
+        <v>125419.52464285713</v>
       </c>
       <c r="E5" s="4">
-        <v>94809.470000000016</v>
+        <v>121329.42096153843</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4">
-        <v>122075.35210526315</v>
+        <v>12732.052631578947</v>
       </c>
       <c r="C6" s="4">
-        <v>95590.301999999996</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4">
-        <v>125419.52464285713</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>121329.42096153843</v>
+        <v>4652.0961538461543</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4">
-        <v>12732.052631578947</v>
+        <v>7170.8421052631575</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>29.6</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
       </c>
       <c r="E7" s="4">
-        <v>4652.0961538461543</v>
+        <v>2622.9615384615386</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4">
-        <v>7170.8421052631575</v>
+        <v>17305.052631578947</v>
       </c>
       <c r="C8" s="4">
-        <v>29.6</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
       </c>
       <c r="E8" s="4">
-        <v>2622.9615384615386</v>
+        <v>6323</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4">
-        <v>17305.052631578947</v>
+        <v>1151.4736842105262</v>
       </c>
       <c r="C9" s="4">
         <v>0</v>
@@ -1927,92 +1923,75 @@
         <v>0</v>
       </c>
       <c r="E9" s="4">
-        <v>6323</v>
+        <v>420.73076923076923</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4">
-        <v>1151.4736842105262</v>
+        <v>7345.6315789473683</v>
       </c>
       <c r="C10" s="4">
-        <v>0</v>
+        <v>16315.8</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>25568.428571428572</v>
       </c>
       <c r="E10" s="4">
-        <v>420.73076923076923</v>
+        <v>18020.423076923078</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
-        <v>7345.6315789473683</v>
+        <v>73369.263157894733</v>
       </c>
       <c r="C11" s="4">
-        <v>16315.8</v>
+        <v>76075.600000000006</v>
       </c>
       <c r="D11" s="4">
-        <v>25568.428571428572</v>
+        <v>93079.071428571435</v>
       </c>
       <c r="E11" s="4">
-        <v>18020.423076923078</v>
+        <v>84242.461538461532</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4">
-        <v>73369.263157894733</v>
+        <v>2260.2105263157896</v>
       </c>
       <c r="C12" s="4">
-        <v>76075.600000000006</v>
+        <v>297.39999999999998</v>
       </c>
       <c r="D12" s="4">
-        <v>93079.071428571435</v>
+        <v>1504</v>
       </c>
       <c r="E12" s="4">
-        <v>84242.461538461532</v>
+        <v>1664.2884615384614</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B13" s="4">
-        <v>2260.2105263157896</v>
+        <v>1852.1226315789474</v>
       </c>
       <c r="C13" s="4">
-        <v>297.39999999999998</v>
+        <v>1482.7840000000001</v>
       </c>
       <c r="D13" s="4">
-        <v>1504</v>
+        <v>1864.4721428571429</v>
       </c>
       <c r="E13" s="4">
-        <v>1664.2884615384614</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="4">
-        <v>35190.33</v>
-      </c>
-      <c r="C14" s="4">
-        <v>7413.92</v>
-      </c>
-      <c r="D14" s="4">
-        <v>52205.22</v>
-      </c>
-      <c r="E14" s="4">
-        <v>94809.470000000016</v>
+        <v>1823.2590384615387</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -2028,7 +2007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
@@ -5265,7 +5244,7 @@
         <v>16</v>
       </c>
       <c r="P8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="5">
         <f>AVERAGE(E2:E20)</f>
@@ -5392,42 +5371,42 @@
         <v>16</v>
       </c>
       <c r="P10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q10" s="5">
-        <f>AVERAGE(E21:E25)</f>
+        <f t="shared" ref="Q10:Y10" si="1">AVERAGE(E21:E25)</f>
         <v>2.936704299473993E-4</v>
       </c>
       <c r="R10" s="5">
-        <f>AVERAGE(F21:F25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S10" s="5">
-        <f>AVERAGE(G21:G25)</f>
+        <f t="shared" si="1"/>
         <v>0.17042351997323815</v>
       </c>
       <c r="T10" s="5">
-        <f>AVERAGE(H21:H25)</f>
+        <f t="shared" si="1"/>
         <v>0.17071719040318553</v>
       </c>
       <c r="U10" s="5">
-        <f>AVERAGE(I21:I25)</f>
+        <f t="shared" si="1"/>
         <v>2.9982624679441388E-2</v>
       </c>
       <c r="V10" s="5">
-        <f>AVERAGE(J21:J25)</f>
+        <f t="shared" si="1"/>
         <v>0.79622802647010027</v>
       </c>
       <c r="W10" s="5">
-        <f>AVERAGE(K21:K25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X10" s="5">
-        <f>AVERAGE(L21:L25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y10" s="5">
-        <f>AVERAGE(M21:M25)</f>
+        <f t="shared" si="1"/>
         <v>3.1389762995099888E-3</v>
       </c>
     </row>
@@ -5519,42 +5498,42 @@
         <v>16</v>
       </c>
       <c r="P12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q12" s="5">
-        <f>AVERAGE(E26:E53)</f>
+        <f t="shared" ref="Q12:Y12" si="2">AVERAGE(E26:E53)</f>
         <v>0</v>
       </c>
       <c r="R12" s="5">
-        <f>AVERAGE(F26:F53)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S12" s="5">
-        <f>AVERAGE(G26:G53)</f>
+        <f t="shared" si="2"/>
         <v>0.2036825180983686</v>
       </c>
       <c r="T12" s="5">
-        <f>AVERAGE(H26:H53)</f>
+        <f t="shared" si="2"/>
         <v>0.2036825180983686</v>
       </c>
       <c r="U12" s="5">
-        <f>AVERAGE(I26:I53)</f>
+        <f t="shared" si="2"/>
         <v>4.1968857133237357E-2</v>
       </c>
       <c r="V12" s="5">
-        <f>AVERAGE(J26:J53)</f>
+        <f t="shared" si="2"/>
         <v>0.74246422756796548</v>
       </c>
       <c r="W12" s="5">
-        <f>AVERAGE(K26:K53)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X12" s="5">
-        <f>AVERAGE(L26:L53)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y12" s="5">
-        <f>AVERAGE(M26:M53)</f>
+        <f t="shared" si="2"/>
         <v>1.1872941413118954E-2</v>
       </c>
     </row>

</xml_diff>